<commit_message>
Updated Instruction Softskill Assessment
Updated Instruction Softskill Assessment
</commit_message>
<xml_diff>
--- a/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Digitale_Kompetenzen.xlsx
+++ b/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Digitale_Kompetenzen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanaBoscolo\source\repos\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42397423-A751-47AF-A6FD-9254A22FC0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E26946-3737-4414-A382-B898AD469C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="31920" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
+    <workbookView xWindow="3930" yWindow="5010" windowWidth="32235" windowHeight="21945" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Booklet_FK Lagerlogistik" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="204">
   <si>
     <t>ItemID</t>
   </si>
@@ -643,6 +643,12 @@
   </si>
   <si>
     <t>Ich nutze, sofern verfügbar, öffentliche WLAN-Netzwerke.</t>
+  </si>
+  <si>
+    <t>Bitte klicke an.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1290,7 +1296,7 @@
   <dimension ref="A1:BO56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AK52" sqref="A51:AK52"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1514,8 +1520,11 @@
       <c r="D2" t="s">
         <v>71</v>
       </c>
+      <c r="E2" t="s">
+        <v>84</v>
+      </c>
       <c r="J2" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L2">
         <v>6</v>
@@ -1575,8 +1584,11 @@
       <c r="D3" t="s">
         <v>72</v>
       </c>
+      <c r="E3" t="s">
+        <v>84</v>
+      </c>
       <c r="J3" t="s">
-        <v>84</v>
+        <v>203</v>
       </c>
       <c r="L3">
         <v>6</v>
@@ -1636,8 +1648,11 @@
       <c r="D4" t="s">
         <v>73</v>
       </c>
+      <c r="E4" t="s">
+        <v>84</v>
+      </c>
       <c r="J4" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L4">
         <v>6</v>
@@ -1697,8 +1712,11 @@
       <c r="D5" t="s">
         <v>74</v>
       </c>
+      <c r="E5" t="s">
+        <v>84</v>
+      </c>
       <c r="J5" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L5">
         <v>6</v>
@@ -1758,8 +1776,11 @@
       <c r="D6" t="s">
         <v>75</v>
       </c>
+      <c r="E6" t="s">
+        <v>84</v>
+      </c>
       <c r="J6" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L6">
         <v>6</v>
@@ -1819,8 +1840,11 @@
       <c r="D7" t="s">
         <v>76</v>
       </c>
+      <c r="E7" t="s">
+        <v>84</v>
+      </c>
       <c r="J7" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L7">
         <v>6</v>
@@ -1880,8 +1904,11 @@
       <c r="D8" t="s">
         <v>77</v>
       </c>
+      <c r="E8" t="s">
+        <v>84</v>
+      </c>
       <c r="J8" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L8">
         <v>6</v>
@@ -1941,8 +1968,11 @@
       <c r="D9" s="8" t="s">
         <v>92</v>
       </c>
+      <c r="E9" t="s">
+        <v>84</v>
+      </c>
       <c r="J9" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L9">
         <v>6</v>
@@ -2000,8 +2030,11 @@
       <c r="D10" t="s">
         <v>93</v>
       </c>
+      <c r="E10" t="s">
+        <v>84</v>
+      </c>
       <c r="J10" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L10">
         <v>6</v>
@@ -2059,8 +2092,11 @@
       <c r="D11" s="9" t="s">
         <v>94</v>
       </c>
+      <c r="E11" t="s">
+        <v>84</v>
+      </c>
       <c r="J11" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L11">
         <v>6</v>
@@ -2118,8 +2154,11 @@
       <c r="D12" s="9" t="s">
         <v>95</v>
       </c>
+      <c r="E12" t="s">
+        <v>84</v>
+      </c>
       <c r="J12" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L12">
         <v>6</v>
@@ -2177,8 +2216,11 @@
       <c r="D13" s="8" t="s">
         <v>96</v>
       </c>
+      <c r="E13" t="s">
+        <v>84</v>
+      </c>
       <c r="J13" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L13">
         <v>6</v>
@@ -2236,8 +2278,11 @@
       <c r="D14" s="8" t="s">
         <v>97</v>
       </c>
+      <c r="E14" t="s">
+        <v>84</v>
+      </c>
       <c r="J14" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L14">
         <v>6</v>
@@ -2295,8 +2340,11 @@
       <c r="D15" s="8" t="s">
         <v>146</v>
       </c>
+      <c r="E15" t="s">
+        <v>84</v>
+      </c>
       <c r="J15" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L15">
         <v>6</v>
@@ -2354,8 +2402,11 @@
       <c r="D16" s="8" t="s">
         <v>147</v>
       </c>
+      <c r="E16" t="s">
+        <v>84</v>
+      </c>
       <c r="J16" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L16">
         <v>6</v>
@@ -2413,8 +2464,11 @@
       <c r="D17" s="8" t="s">
         <v>148</v>
       </c>
+      <c r="E17" t="s">
+        <v>84</v>
+      </c>
       <c r="J17" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L17">
         <v>6</v>
@@ -2472,8 +2526,11 @@
       <c r="D18" s="10" t="s">
         <v>149</v>
       </c>
+      <c r="E18" t="s">
+        <v>84</v>
+      </c>
       <c r="J18" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L18">
         <v>6</v>
@@ -2531,8 +2588,11 @@
       <c r="D19" s="11" t="s">
         <v>150</v>
       </c>
+      <c r="E19" t="s">
+        <v>84</v>
+      </c>
       <c r="J19" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L19">
         <v>6</v>
@@ -2590,8 +2650,11 @@
       <c r="D20" s="8" t="s">
         <v>151</v>
       </c>
+      <c r="E20" t="s">
+        <v>84</v>
+      </c>
       <c r="J20" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L20">
         <v>6</v>
@@ -2649,8 +2712,11 @@
       <c r="D21" s="8" t="s">
         <v>152</v>
       </c>
+      <c r="E21" t="s">
+        <v>84</v>
+      </c>
       <c r="J21" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L21">
         <v>6</v>
@@ -2708,8 +2774,11 @@
       <c r="D22" s="11" t="s">
         <v>153</v>
       </c>
+      <c r="E22" t="s">
+        <v>84</v>
+      </c>
       <c r="J22" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L22">
         <v>6</v>
@@ -2767,8 +2836,11 @@
       <c r="D23" s="14" t="s">
         <v>168</v>
       </c>
+      <c r="E23" t="s">
+        <v>84</v>
+      </c>
       <c r="J23" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L23">
         <v>6</v>
@@ -2826,8 +2898,11 @@
       <c r="D24" s="14" t="s">
         <v>169</v>
       </c>
+      <c r="E24" t="s">
+        <v>84</v>
+      </c>
       <c r="J24" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L24">
         <v>6</v>
@@ -2885,8 +2960,11 @@
       <c r="D25" s="14" t="s">
         <v>170</v>
       </c>
+      <c r="E25" t="s">
+        <v>84</v>
+      </c>
       <c r="J25" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L25">
         <v>6</v>
@@ -2944,8 +3022,11 @@
       <c r="D26" s="14" t="s">
         <v>171</v>
       </c>
+      <c r="E26" t="s">
+        <v>84</v>
+      </c>
       <c r="J26" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L26">
         <v>6</v>
@@ -3003,8 +3084,11 @@
       <c r="D27" s="14" t="s">
         <v>172</v>
       </c>
+      <c r="E27" t="s">
+        <v>84</v>
+      </c>
       <c r="J27" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L27">
         <v>6</v>
@@ -3062,8 +3146,11 @@
       <c r="D28" s="14" t="s">
         <v>173</v>
       </c>
+      <c r="E28" t="s">
+        <v>84</v>
+      </c>
       <c r="J28" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L28">
         <v>6</v>
@@ -3121,8 +3208,11 @@
       <c r="D29" s="14" t="s">
         <v>174</v>
       </c>
+      <c r="E29" t="s">
+        <v>84</v>
+      </c>
       <c r="J29" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L29">
         <v>6</v>
@@ -3180,8 +3270,11 @@
       <c r="D30" s="15" t="s">
         <v>175</v>
       </c>
+      <c r="E30" t="s">
+        <v>84</v>
+      </c>
       <c r="J30" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L30">
         <v>6</v>
@@ -3239,8 +3332,11 @@
       <c r="D31" s="14" t="s">
         <v>176</v>
       </c>
+      <c r="E31" t="s">
+        <v>84</v>
+      </c>
       <c r="J31" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L31">
         <v>6</v>
@@ -3298,8 +3394,11 @@
       <c r="D32" s="14" t="s">
         <v>177</v>
       </c>
+      <c r="E32" t="s">
+        <v>84</v>
+      </c>
       <c r="J32" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L32">
         <v>6</v>
@@ -3357,8 +3456,11 @@
       <c r="D33" s="8" t="s">
         <v>178</v>
       </c>
+      <c r="E33" t="s">
+        <v>84</v>
+      </c>
       <c r="J33" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L33">
         <v>6</v>
@@ -3416,8 +3518,11 @@
       <c r="D34" s="11" t="s">
         <v>179</v>
       </c>
+      <c r="E34" t="s">
+        <v>84</v>
+      </c>
       <c r="J34" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L34">
         <v>6</v>
@@ -3475,8 +3580,11 @@
       <c r="D35" s="8" t="s">
         <v>180</v>
       </c>
+      <c r="E35" t="s">
+        <v>84</v>
+      </c>
       <c r="J35" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L35">
         <v>6</v>
@@ -3534,8 +3642,11 @@
       <c r="D36" s="8" t="s">
         <v>181</v>
       </c>
+      <c r="E36" t="s">
+        <v>84</v>
+      </c>
       <c r="J36" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L36">
         <v>6</v>
@@ -3593,8 +3704,11 @@
       <c r="D37" s="8" t="s">
         <v>182</v>
       </c>
+      <c r="E37" t="s">
+        <v>84</v>
+      </c>
       <c r="J37" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L37">
         <v>6</v>
@@ -3652,8 +3766,11 @@
       <c r="D38" s="8" t="s">
         <v>183</v>
       </c>
+      <c r="E38" t="s">
+        <v>84</v>
+      </c>
       <c r="J38" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L38">
         <v>6</v>
@@ -3711,8 +3828,11 @@
       <c r="D39" s="11" t="s">
         <v>184</v>
       </c>
+      <c r="E39" t="s">
+        <v>84</v>
+      </c>
       <c r="J39" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L39">
         <v>6</v>
@@ -3770,8 +3890,11 @@
       <c r="D40" s="16" t="s">
         <v>185</v>
       </c>
+      <c r="E40" t="s">
+        <v>84</v>
+      </c>
       <c r="J40" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L40">
         <v>6</v>
@@ -3829,8 +3952,11 @@
       <c r="D41" s="10" t="s">
         <v>186</v>
       </c>
+      <c r="E41" t="s">
+        <v>84</v>
+      </c>
       <c r="J41" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L41">
         <v>6</v>
@@ -3888,8 +4014,11 @@
       <c r="D42" s="8" t="s">
         <v>187</v>
       </c>
+      <c r="E42" t="s">
+        <v>84</v>
+      </c>
       <c r="J42" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L42">
         <v>6</v>
@@ -3947,8 +4076,11 @@
       <c r="D43" s="8" t="s">
         <v>188</v>
       </c>
+      <c r="E43" t="s">
+        <v>84</v>
+      </c>
       <c r="J43" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L43">
         <v>6</v>
@@ -4006,8 +4138,11 @@
       <c r="D44" s="8" t="s">
         <v>189</v>
       </c>
+      <c r="E44" t="s">
+        <v>84</v>
+      </c>
       <c r="J44" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L44">
         <v>6</v>
@@ -4065,8 +4200,11 @@
       <c r="D45" s="8" t="s">
         <v>190</v>
       </c>
+      <c r="E45" t="s">
+        <v>84</v>
+      </c>
       <c r="J45" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L45">
         <v>6</v>
@@ -4124,8 +4262,11 @@
       <c r="D46" s="8" t="s">
         <v>191</v>
       </c>
+      <c r="E46" t="s">
+        <v>84</v>
+      </c>
       <c r="J46" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L46">
         <v>6</v>
@@ -4183,8 +4324,11 @@
       <c r="D47" s="8" t="s">
         <v>192</v>
       </c>
+      <c r="E47" t="s">
+        <v>84</v>
+      </c>
       <c r="J47" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L47">
         <v>6</v>
@@ -4242,8 +4386,11 @@
       <c r="D48" s="8" t="s">
         <v>193</v>
       </c>
+      <c r="E48" t="s">
+        <v>84</v>
+      </c>
       <c r="J48" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L48">
         <v>6</v>
@@ -4301,8 +4448,11 @@
       <c r="D49" s="8" t="s">
         <v>199</v>
       </c>
+      <c r="E49" t="s">
+        <v>84</v>
+      </c>
       <c r="J49" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L49">
         <v>6</v>
@@ -4360,8 +4510,11 @@
       <c r="D50" s="8" t="s">
         <v>194</v>
       </c>
+      <c r="E50" t="s">
+        <v>84</v>
+      </c>
       <c r="J50" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L50">
         <v>6</v>
@@ -4419,8 +4572,11 @@
       <c r="D51" s="16" t="s">
         <v>200</v>
       </c>
+      <c r="E51" t="s">
+        <v>84</v>
+      </c>
       <c r="J51" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L51">
         <v>6</v>
@@ -4478,8 +4634,11 @@
       <c r="D52" s="8" t="s">
         <v>201</v>
       </c>
+      <c r="E52" t="s">
+        <v>84</v>
+      </c>
       <c r="J52" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L52">
         <v>6</v>
@@ -4537,8 +4696,11 @@
       <c r="D53" s="11" t="s">
         <v>195</v>
       </c>
+      <c r="E53" t="s">
+        <v>84</v>
+      </c>
       <c r="J53" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L53">
         <v>6</v>
@@ -4596,8 +4758,11 @@
       <c r="D54" s="8" t="s">
         <v>196</v>
       </c>
+      <c r="E54" t="s">
+        <v>84</v>
+      </c>
       <c r="J54" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L54">
         <v>6</v>
@@ -4655,8 +4820,11 @@
       <c r="D55" s="8" t="s">
         <v>197</v>
       </c>
+      <c r="E55" t="s">
+        <v>84</v>
+      </c>
       <c r="J55" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L55">
         <v>6</v>
@@ -4714,8 +4882,11 @@
       <c r="D56" s="8" t="s">
         <v>198</v>
       </c>
+      <c r="E56" t="s">
+        <v>84</v>
+      </c>
       <c r="J56" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="L56">
         <v>6</v>
@@ -4831,17 +5002,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02625a54-df84-4a3b-b049-0bb7e92cde0d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100879B58D3C23DCA4AAEF47596CA4D8E48" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ee8b9d8723b80ccc4cb578ffd4faacc7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="02625a54-df84-4a3b-b049-0bb7e92cde0d" xmlns:ns3="c90f9e10-81f0-426e-b8bb-fc89022b3796" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64b8ed4db9a6e136c161da669116b9cc" ns2:_="" ns3:_="">
     <xsd:import namespace="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
@@ -5050,6 +5210,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02625a54-df84-4a3b-b049-0bb7e92cde0d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5060,23 +5231,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A223085B-57B4-40DB-BC96-92703C914FDC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5095,6 +5249,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
   <ds:schemaRefs>

</xml_diff>